<commit_message>
update review with PGx team
</commit_message>
<xml_diff>
--- a/validation/results/105/105.xlsx
+++ b/validation/results/105/105.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="peak_table" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,14 +12,14 @@
     <sheet name="genotype_result" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -29,24 +28,20 @@
       <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <name val="돋움"/>
+      <charset val="129"/>
+      <family val="3"/>
+      <sz val="8"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Cambria"/>
-      <charset val="1"/>
-      <family val="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -62,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -71,10 +66,33 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -84,42 +102,25 @@
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -476,1175 +477,1174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P10" activeCellId="0" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col width="10.58" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.21" customWidth="1" style="2" min="3" max="3"/>
-    <col width="12.35" customWidth="1" style="2" min="4" max="4"/>
+    <col width="10.54296875" customWidth="1" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" min="3" max="3"/>
+    <col width="12.36328125" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="3">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>panel</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>gene</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>marker_label</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>marker</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>is_forward</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>w_min</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>w_max</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>m_min</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>m_max</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>w_base</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>m_base</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>w_color</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>m_color</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>w_height</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>m_height</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="3">
-      <c r="A2" s="2" t="inlineStr">
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" t="inlineStr">
         <is>
           <t>S1</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>CYP2D6_14</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>CYP2D6_001</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" t="n">
         <v>25</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" t="n">
         <v>35</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" t="n">
         <v>27</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" t="n">
         <v>36</v>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>blue</t>
         </is>
       </c>
-      <c r="M2" s="2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>green</t>
         </is>
       </c>
-      <c r="N2" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O2" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" ht="15" customHeight="1" s="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="N2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="inlineStr">
         <is>
           <t>S1</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>CYP2D6_10B</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>CYP2D6_002</t>
         </is>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" t="n">
         <v>28</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" t="n">
         <v>38</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" t="n">
         <v>31</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" t="n">
         <v>37</v>
       </c>
-      <c r="J3" s="2" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="K3" s="2" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="L3" s="2" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>black</t>
         </is>
       </c>
-      <c r="M3" s="2" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>red</t>
         </is>
       </c>
-      <c r="N3" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O3" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="3">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="N3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="inlineStr">
         <is>
           <t>S1</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>CYP2D6_49</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>CYP2D6_003</t>
         </is>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" t="n">
         <v>37</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" t="n">
         <v>44</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" t="n">
         <v>39</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="I4" t="n">
         <v>45</v>
       </c>
-      <c r="J4" s="2" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>T</t>
         </is>
       </c>
-      <c r="K4" s="2" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="L4" s="2" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>green</t>
         </is>
       </c>
-      <c r="M4" s="2" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>red</t>
         </is>
       </c>
-      <c r="N4" s="2" t="n">
+      <c r="N4" t="n">
+        <v>800</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CYP2D6_21</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CYP2D6_004</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>41</v>
+      </c>
+      <c r="G5" t="n">
+        <v>45</v>
+      </c>
+      <c r="H5" t="n">
+        <v>42</v>
+      </c>
+      <c r="I5" t="n">
+        <v>49</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>black</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CYP2D6_41</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CYP2D6_005</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>45</v>
+      </c>
+      <c r="G6" t="n">
+        <v>50</v>
+      </c>
+      <c r="H6" t="n">
+        <v>47</v>
+      </c>
+      <c r="I6" t="n">
+        <v>50</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
         <v>700</v>
       </c>
-      <c r="O4" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" s="3">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="O6" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="inlineStr">
         <is>
           <t>S1</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_21</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_004</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CYP2D6_52</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CYP2D6_006</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>50</v>
+      </c>
+      <c r="G7" t="n">
+        <v>53</v>
+      </c>
+      <c r="H7" t="n">
+        <v>50</v>
+      </c>
+      <c r="I7" t="n">
+        <v>55</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>black</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CYP2D6_18</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>CYP2D6_007</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F8" t="n">
+        <v>53</v>
+      </c>
+      <c r="G8" t="n">
+        <v>57</v>
+      </c>
+      <c r="H8" t="n">
+        <v>55</v>
+      </c>
+      <c r="I8" t="n">
+        <v>59</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>500</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CYP2D6_2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>CYP2D6_008</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>57</v>
+      </c>
+      <c r="G9" t="n">
+        <v>62</v>
+      </c>
+      <c r="H9" t="n">
+        <v>59</v>
+      </c>
+      <c r="I9" t="n">
+        <v>63</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CYP2D6_60</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>CYP2D6_009</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>63</v>
+      </c>
+      <c r="G10" t="n">
+        <v>68</v>
+      </c>
+      <c r="H10" t="n">
+        <v>65</v>
+      </c>
+      <c r="I10" t="n">
+        <v>68</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>black</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CYP2D6_5</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>CYP2D6_010</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>68</v>
+      </c>
+      <c r="G11" t="n">
+        <v>73</v>
+      </c>
+      <c r="H11" t="n">
+        <v>68</v>
+      </c>
+      <c r="I11" t="n">
+        <v>72</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>black</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CYP2D6_4</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>CYP2D6_011</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>26</v>
+      </c>
+      <c r="G12" t="n">
+        <v>32</v>
+      </c>
+      <c r="H12" t="n">
+        <v>29</v>
+      </c>
+      <c r="I12" t="n">
+        <v>34</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CYP2D6_3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>CYP2D6_012</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>33</v>
+      </c>
+      <c r="G13" t="n">
+        <v>38</v>
+      </c>
+      <c r="H13" t="n">
+        <v>32</v>
+      </c>
+      <c r="I13" t="n">
+        <v>36</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CYP2D6_17</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>CYP2D6_013</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>36</v>
+      </c>
+      <c r="G14" t="n">
         <v>41</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="H14" t="n">
+        <v>38</v>
+      </c>
+      <c r="I14" t="n">
+        <v>43</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>black</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>CYP2D6_9</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>CYP2D6_014</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>41</v>
+      </c>
+      <c r="G15" t="n">
+        <v>46</v>
+      </c>
+      <c r="H15" t="n">
+        <v>39</v>
+      </c>
+      <c r="I15" t="n">
         <v>45</v>
       </c>
-      <c r="H5" s="2" t="n">
-        <v>42</v>
-      </c>
-      <c r="I5" s="2" t="n">
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>CYP2D6_6</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>CYP2D6_015</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>45</v>
+      </c>
+      <c r="G16" t="n">
         <v>49</v>
       </c>
-      <c r="J5" s="2" t="inlineStr">
+      <c r="H16" t="n">
+        <v>46</v>
+      </c>
+      <c r="I16" t="n">
+        <v>49</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="K5" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="L5" s="2" t="inlineStr">
-        <is>
-          <t>blue</t>
-        </is>
-      </c>
-      <c r="M5" s="2" t="inlineStr">
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
         <is>
           <t>black</t>
         </is>
       </c>
-      <c r="N5" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O5" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1" s="3">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_41</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_005</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="G6" s="2" t="n">
+      <c r="N16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O16" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CYP2D6_29</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>CYP2D6_016</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
         <v>50</v>
       </c>
-      <c r="H6" s="2" t="n">
-        <v>47</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="J6" s="2" t="inlineStr">
+      <c r="G17" t="n">
+        <v>55</v>
+      </c>
+      <c r="H17" t="n">
+        <v>52</v>
+      </c>
+      <c r="I17" t="n">
+        <v>57</v>
+      </c>
+      <c r="J17" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="K6" s="2" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="L6" s="2" t="inlineStr">
-        <is>
-          <t>blue</t>
-        </is>
-      </c>
-      <c r="M6" s="2" t="inlineStr">
-        <is>
-          <t>green</t>
-        </is>
-      </c>
-      <c r="N6" s="2" t="n">
-        <v>700</v>
-      </c>
-      <c r="O6" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1" s="3">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_52</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_006</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="n">
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>black</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>red</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CYP2D6</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>CYP2D6_XN</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>CYP2D6_017</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>53</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>55</v>
-      </c>
-      <c r="J7" s="2" t="inlineStr">
+      <c r="F18" t="n">
+        <v>66</v>
+      </c>
+      <c r="G18" t="n">
+        <v>73</v>
+      </c>
+      <c r="H18" t="n">
+        <v>70</v>
+      </c>
+      <c r="I18" t="n">
+        <v>75</v>
+      </c>
+      <c r="J18" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="K7" s="2" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="L7" s="2" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>black</t>
         </is>
       </c>
-      <c r="M7" s="2" t="inlineStr">
+      <c r="M18" t="inlineStr">
         <is>
           <t>red</t>
         </is>
       </c>
-      <c r="N7" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O7" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1" s="3">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_18</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_007</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>53</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>57</v>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>55</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>59</v>
-      </c>
-      <c r="J8" s="2" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="K8" s="2" t="inlineStr">
-        <is>
-          <t>T</t>
-        </is>
-      </c>
-      <c r="L8" s="2" t="inlineStr">
-        <is>
-          <t>blue</t>
-        </is>
-      </c>
-      <c r="M8" s="2" t="inlineStr">
-        <is>
-          <t>red</t>
-        </is>
-      </c>
-      <c r="N8" s="2" t="n">
-        <v>500</v>
-      </c>
-      <c r="O8" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1" s="3">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_2</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_008</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>57</v>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>62</v>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>59</v>
-      </c>
-      <c r="I9" s="2" t="n">
-        <v>63</v>
-      </c>
-      <c r="J9" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="K9" s="2" t="inlineStr">
-        <is>
-          <t>T</t>
-        </is>
-      </c>
-      <c r="L9" s="2" t="inlineStr">
-        <is>
-          <t>blue</t>
-        </is>
-      </c>
-      <c r="M9" s="2" t="inlineStr">
-        <is>
-          <t>green</t>
-        </is>
-      </c>
-      <c r="N9" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O9" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1" s="3">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_60</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_009</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>63</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>68</v>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>65</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>68</v>
-      </c>
-      <c r="J10" s="2" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="L10" s="2" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-      <c r="M10" s="2" t="inlineStr">
-        <is>
-          <t>red</t>
-        </is>
-      </c>
-      <c r="N10" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O10" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" ht="15" customHeight="1" s="3">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_5</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_010</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>68</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <v>73</v>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>68</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>72</v>
-      </c>
-      <c r="J11" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="K11" s="2" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="L11" s="2" t="inlineStr">
-        <is>
-          <t>red</t>
-        </is>
-      </c>
-      <c r="M11" s="2" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-      <c r="N11" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O11" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1" s="3">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_4</t>
-        </is>
-      </c>
-      <c r="D12" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_011</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="I12" s="2" t="n">
-        <v>34</v>
-      </c>
-      <c r="J12" s="2" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="L12" s="2" t="inlineStr">
-        <is>
-          <t>blue</t>
-        </is>
-      </c>
-      <c r="M12" s="2" t="inlineStr">
-        <is>
-          <t>green</t>
-        </is>
-      </c>
-      <c r="N12" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O12" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="13" ht="15" customHeight="1" s="3">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_3</t>
-        </is>
-      </c>
-      <c r="D13" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_012</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <v>33</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>38</v>
-      </c>
-      <c r="H13" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="I13" s="2" t="n">
-        <v>36</v>
-      </c>
-      <c r="J13" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="L13" s="2" t="inlineStr">
-        <is>
-          <t>green</t>
-        </is>
-      </c>
-      <c r="M13" s="2" t="inlineStr">
-        <is>
-          <t>blue</t>
-        </is>
-      </c>
-      <c r="N13" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O13" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="14" ht="15" customHeight="1" s="3">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_17</t>
-        </is>
-      </c>
-      <c r="D14" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_013</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2" t="n">
-        <v>36</v>
-      </c>
-      <c r="G14" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>38</v>
-      </c>
-      <c r="I14" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="J14" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="inlineStr">
-        <is>
-          <t>T</t>
-        </is>
-      </c>
-      <c r="L14" s="2" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-      <c r="M14" s="2" t="inlineStr">
-        <is>
-          <t>red</t>
-        </is>
-      </c>
-      <c r="N14" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O14" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="15" ht="15" customHeight="1" s="3">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_9</t>
-        </is>
-      </c>
-      <c r="D15" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_014</t>
-        </is>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="H15" s="2" t="n">
-        <v>39</v>
-      </c>
-      <c r="I15" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="J15" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="K15" s="2" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="L15" s="2" t="inlineStr">
-        <is>
-          <t>green</t>
-        </is>
-      </c>
-      <c r="M15" s="2" t="inlineStr">
-        <is>
-          <t>blue</t>
-        </is>
-      </c>
-      <c r="N15" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O15" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="16" ht="15" customHeight="1" s="3">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_6</t>
-        </is>
-      </c>
-      <c r="D16" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_015</t>
-        </is>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2" t="n">
-        <v>45</v>
-      </c>
-      <c r="G16" s="2" t="n">
-        <v>49</v>
-      </c>
-      <c r="H16" s="2" t="n">
-        <v>46</v>
-      </c>
-      <c r="I16" s="2" t="n">
-        <v>49</v>
-      </c>
-      <c r="J16" s="2" t="inlineStr">
-        <is>
-          <t>T</t>
-        </is>
-      </c>
-      <c r="K16" s="2" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="L16" s="2" t="inlineStr">
-        <is>
-          <t>green</t>
-        </is>
-      </c>
-      <c r="M16" s="2" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-      <c r="N16" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O16" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="17" ht="15" customHeight="1" s="3">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_29</t>
-        </is>
-      </c>
-      <c r="D17" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_016</t>
-        </is>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="G17" s="2" t="n">
-        <v>55</v>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>52</v>
-      </c>
-      <c r="I17" s="2" t="n">
-        <v>57</v>
-      </c>
-      <c r="J17" s="2" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="K17" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="L17" s="2" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-      <c r="M17" s="2" t="inlineStr">
-        <is>
-          <t>red</t>
-        </is>
-      </c>
-      <c r="N17" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O17" s="2" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="18" ht="15" customHeight="1" s="3">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_XN</t>
-        </is>
-      </c>
-      <c r="D18" s="2" t="inlineStr">
-        <is>
-          <t>CYP2D6_017</t>
-        </is>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>66</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>73</v>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>70</v>
-      </c>
-      <c r="I18" s="2" t="n">
-        <v>75</v>
-      </c>
-      <c r="J18" s="2" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="K18" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="L18" s="2" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-      <c r="M18" s="2" t="inlineStr">
-        <is>
-          <t>red</t>
-        </is>
-      </c>
-      <c r="N18" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="O18" s="2" t="n">
+      <c r="N18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O18" t="n">
         <v>1000</v>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup orientation="portrait" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -1663,97 +1663,97 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>gene</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>marker</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>panel</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>direction</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>base</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>basetype</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>min_bin</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>max_bin</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>min_height</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>is_forward</t>
         </is>
       </c>
-      <c r="M1" s="5" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>is_detected</t>
         </is>
       </c>
-      <c r="N1" s="5" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>peak</t>
         </is>
       </c>
-      <c r="O1" s="5" t="inlineStr">
+      <c r="O1" s="3" t="inlineStr">
         <is>
           <t>size</t>
         </is>
       </c>
-      <c r="P1" s="5" t="inlineStr">
+      <c r="P1" s="3" t="inlineStr">
         <is>
           <t>height</t>
         </is>
       </c>
-      <c r="Q1" s="5" t="inlineStr">
+      <c r="Q1" s="3" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="R1" s="5" t="inlineStr">
+      <c r="R1" s="3" t="inlineStr">
         <is>
           <t>message</t>
         </is>
       </c>
-      <c r="S1" s="5" t="inlineStr">
+      <c r="S1" s="3" t="inlineStr">
         <is>
           <t>color</t>
         </is>
@@ -2103,7 +2103,7 @@
         <v>44</v>
       </c>
       <c r="K6" t="n">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -4295,42 +4295,42 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>gene</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>marker</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>panel</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>direction</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>genotype</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>phenotype</t>
         </is>
@@ -5070,12 +5070,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>genotype</t>
         </is>

</xml_diff>